<commit_message>
adds treatment costs components
</commit_message>
<xml_diff>
--- a/src/data/data-raw/export_template.xlsx
+++ b/src/data/data-raw/export_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanhoang/FlowWest/SAFER/step-zero-cost-estimator/src/data/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A558C335-03C7-ED4E-8037-83BD1B0BFCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4565AE9B-4E1C-1246-8402-6A83EBA1BFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -246,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -408,43 +408,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -459,15 +428,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -646,6 +606,34 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -657,45 +645,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -748,18 +697,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -829,189 +849,139 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1026,9 +996,96 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1244,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M957"/>
+  <dimension ref="A1:M958"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1265,545 +1322,559 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="4" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="5"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="11"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="12">
+      <c r="I3" s="84"/>
+      <c r="J3" s="11">
         <v>1000002</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="11"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="9" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="88" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="9" t="s">
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="12">
+      <c r="I4" s="84"/>
+      <c r="J4" s="11">
         <v>85</v>
       </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="11"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="11"/>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19" t="s">
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="20"/>
+      <c r="M6" s="19"/>
     </row>
     <row r="7" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="14"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="21" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="20"/>
+      <c r="M7" s="19"/>
     </row>
     <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="21" t="s">
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="20"/>
+      <c r="M8" s="19"/>
     </row>
     <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>6</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="24">
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="23">
         <v>375</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="22">
         <f t="shared" ref="H9" si="0">A9*G9</f>
         <v>2250</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="23">
         <v>20</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="24">
         <f t="shared" ref="J9" si="1">H9/I9</f>
         <v>112.5</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="24">
         <f t="shared" ref="K9" si="2">J9/12</f>
         <v>9.375</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="24">
         <f>K9/J4</f>
         <v>0.11029411764705882</v>
       </c>
-      <c r="M9" s="20"/>
+      <c r="M9" s="19"/>
     </row>
-    <row r="10" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32" t="s">
+    <row r="10" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="20"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="19"/>
     </row>
-    <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34" t="s">
+    <row r="11" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29"/>
+      <c r="B11" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39">
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="31">
         <f>SUM(H9:H10)</f>
         <v>2250</v>
       </c>
-      <c r="I11" s="40"/>
-      <c r="J11" s="86">
+      <c r="I11" s="32"/>
+      <c r="J11" s="65">
         <f>SUM(J9:J10)</f>
         <v>112.5</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K11" s="33">
         <f>SUM(K9:K10)</f>
         <v>9.375</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="33">
         <f>SUM(L9:L10)</f>
         <v>0.11029411764705882</v>
       </c>
-      <c r="M11" s="20"/>
+      <c r="M11" s="19"/>
     </row>
-    <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="42"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="20"/>
+    <row r="12" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="97"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="19"/>
     </row>
-    <row r="13" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="47"/>
-      <c r="B13" s="48" t="s">
+    <row r="13" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="38"/>
+      <c r="B13" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="20"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="76">
+      <c r="A14" s="61">
         <v>1</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="80">
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="62">
         <v>350000</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="22">
         <f t="shared" ref="H14" si="3">A14*G14</f>
         <v>350000</v>
       </c>
-      <c r="I14" s="80">
+      <c r="I14" s="62">
         <v>45</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="24">
         <f t="shared" ref="J14" si="4">H14/I14</f>
         <v>7777.7777777777774</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="24">
         <f t="shared" ref="K14" si="5">J14/12</f>
         <v>648.14814814814815</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="24">
         <f>K14/J4</f>
         <v>7.6252723311546839</v>
       </c>
-      <c r="M14" s="20"/>
+      <c r="M14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="81"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="20"/>
+    <row r="15" spans="1:13" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="63"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="19"/>
     </row>
-    <row r="16" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52" t="s">
+    <row r="16" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40"/>
+      <c r="B16" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="55">
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="108"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="42">
         <f>SUM(H14:H14)</f>
         <v>350000</v>
       </c>
-      <c r="I16" s="56" t="s">
+      <c r="I16" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="J16" s="87">
+      <c r="J16" s="66">
         <f>SUM(J14:J14)</f>
         <v>7777.7777777777774</v>
       </c>
-      <c r="K16" s="57">
+      <c r="K16" s="44">
         <f>SUM(K14:K14)</f>
         <v>648.14814814814815</v>
       </c>
-      <c r="L16" s="58">
+      <c r="L16" s="45">
         <f>SUM(L14:L14)</f>
         <v>7.6252723311546839</v>
       </c>
-      <c r="M16" s="20"/>
+      <c r="M16" s="19"/>
     </row>
-    <row r="17" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="42"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="20"/>
+    <row r="17" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="19"/>
     </row>
-    <row r="18" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="14"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="62" t="s">
+    <row r="18" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="64">
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="49">
         <f>SUM(H11,H16)</f>
         <v>352250</v>
       </c>
-      <c r="I18" s="65"/>
-      <c r="J18" s="64">
+      <c r="I18" s="50"/>
+      <c r="J18" s="49">
         <f>SUM(J11,J16)</f>
         <v>7890.2777777777774</v>
       </c>
-      <c r="K18" s="66">
+      <c r="K18" s="51">
         <f>SUM(K11,K16)</f>
         <v>657.52314814814815</v>
       </c>
-      <c r="L18" s="64">
+      <c r="L18" s="49">
         <f>SUM(L11,L16)</f>
         <v>7.7355664488017428</v>
       </c>
-      <c r="M18" s="20"/>
+      <c r="M18" s="19"/>
     </row>
     <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="14"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="20"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="19"/>
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="14"/>
-      <c r="B20" s="18" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18" t="s">
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="L20" s="18"/>
-      <c r="M20" s="20"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="19"/>
     </row>
-    <row r="21" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="67"/>
-      <c r="B21" s="68"/>
-      <c r="C21" s="68" t="s">
+    <row r="21" spans="1:13" s="67" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="13"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="19"/>
+    </row>
+    <row r="22" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="52"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
-      <c r="M21" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="54"/>
     </row>
-    <row r="22" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="70"/>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="70"/>
-      <c r="M22" s="70"/>
-    </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="91" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="92"/>
-      <c r="C23" s="92"/>
-      <c r="D23" s="92"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="92"/>
-      <c r="G23" s="92"/>
-      <c r="H23" s="92"/>
-      <c r="I23" s="92"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="92"/>
-      <c r="L23" s="92"/>
-      <c r="M23" s="93"/>
+    <row r="23" spans="1:13" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="55"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
     </row>
     <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="94"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="95"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
-      <c r="J24" s="95"/>
-      <c r="K24" s="95"/>
-      <c r="L24" s="95"/>
-      <c r="M24" s="96"/>
+      <c r="A24" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="76"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="94"/>
-      <c r="B25" s="95"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="95"/>
-      <c r="I25" s="95"/>
-      <c r="J25" s="95"/>
-      <c r="K25" s="95"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="96"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="79"/>
     </row>
-    <row r="26" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="97"/>
-      <c r="B26" s="98"/>
-      <c r="C26" s="98"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="F26" s="98"/>
-      <c r="G26" s="98"/>
-      <c r="H26" s="98"/>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="98"/>
-      <c r="M26" s="99"/>
+    <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="77"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="79"/>
     </row>
-    <row r="27" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="80"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="81"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="82"/>
+    </row>
     <row r="28" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="29" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="30" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2734,10 +2805,28 @@
     <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="19">
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="B1:H1"/>
     <mergeCell ref="D4:G4"/>
-    <mergeCell ref="A23:M26"/>
+    <mergeCell ref="A24:M27"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>